<commit_message>
better validation for aviation
</commit_message>
<xml_diff>
--- a/examples/programs/all_programs.xlsx
+++ b/examples/programs/all_programs.xlsx
@@ -1600,10 +1600,10 @@
       <c r="AH2" t="n">
         <v>0.0165</v>
       </c>
-      <c r="AM2" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN2" t="b">
+      <c r="AM2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN2" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1631,10 +1631,10 @@
       <c r="AH3" t="n">
         <v>0.0165</v>
       </c>
-      <c r="AM3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN3" t="b">
+      <c r="AM3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1662,10 +1662,10 @@
       <c r="AH4" t="n">
         <v>0.0165</v>
       </c>
-      <c r="AM4" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN4" t="b">
+      <c r="AM4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1693,10 +1693,10 @@
       <c r="AH5" t="n">
         <v>0.0165</v>
       </c>
-      <c r="AM5" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN5" t="b">
+      <c r="AM5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1724,10 +1724,10 @@
       <c r="AH6" t="n">
         <v>0.0165</v>
       </c>
-      <c r="AM6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN6" t="b">
+      <c r="AM6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN6" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1755,10 +1755,10 @@
       <c r="AH7" t="n">
         <v>0.05</v>
       </c>
-      <c r="AM7" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN7" t="b">
+      <c r="AM7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1786,10 +1786,10 @@
       <c r="AH8" t="n">
         <v>0.05</v>
       </c>
-      <c r="AM8" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN8" t="b">
+      <c r="AM8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN8" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1817,10 +1817,10 @@
       <c r="AH9" t="n">
         <v>0.05</v>
       </c>
-      <c r="AM9" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN9" t="b">
+      <c r="AM9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN9" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1848,10 +1848,10 @@
       <c r="AH10" t="n">
         <v>0.05</v>
       </c>
-      <c r="AM10" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN10" t="b">
+      <c r="AM10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN10" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1879,10 +1879,10 @@
       <c r="AH11" t="n">
         <v>0.05</v>
       </c>
-      <c r="AM11" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN11" t="b">
+      <c r="AM11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN11" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1910,10 +1910,10 @@
       <c r="AH12" t="n">
         <v>0.05</v>
       </c>
-      <c r="AM12" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN12" t="b">
+      <c r="AM12" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN12" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1941,10 +1941,10 @@
       <c r="AH13" t="n">
         <v>0.05</v>
       </c>
-      <c r="AM13" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN13" t="b">
+      <c r="AM13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN13" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1972,10 +1972,10 @@
       <c r="AH14" t="n">
         <v>0.05</v>
       </c>
-      <c r="AM14" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN14" t="b">
+      <c r="AM14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN14" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2003,10 +2003,10 @@
       <c r="AH15" t="n">
         <v>0.05</v>
       </c>
-      <c r="AM15" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN15" t="b">
+      <c r="AM15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN15" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2034,10 +2034,10 @@
       <c r="AH16" t="n">
         <v>0.05</v>
       </c>
-      <c r="AM16" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN16" t="b">
+      <c r="AM16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN16" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2065,10 +2065,10 @@
       <c r="AH17" t="n">
         <v>0.05</v>
       </c>
-      <c r="AM17" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN17" t="b">
+      <c r="AM17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN17" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2096,10 +2096,10 @@
       <c r="AH18" t="n">
         <v>0.05</v>
       </c>
-      <c r="AM18" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN18" t="b">
+      <c r="AM18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN18" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2127,10 +2127,10 @@
       <c r="AH19" t="n">
         <v>0.05</v>
       </c>
-      <c r="AM19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN19" t="b">
+      <c r="AM19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN19" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2158,10 +2158,10 @@
       <c r="AH20" t="n">
         <v>0.05</v>
       </c>
-      <c r="AM20" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN20" t="b">
+      <c r="AM20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN20" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2189,10 +2189,10 @@
       <c r="AH21" t="n">
         <v>0.05</v>
       </c>
-      <c r="AM21" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN21" t="b">
+      <c r="AM21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN21" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2220,10 +2220,10 @@
       <c r="AH22" t="n">
         <v>0.05</v>
       </c>
-      <c r="AM22" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN22" t="b">
+      <c r="AM22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN22" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2251,10 +2251,10 @@
       <c r="AH23" t="n">
         <v>0.05</v>
       </c>
-      <c r="AM23" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN23" t="b">
+      <c r="AM23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN23" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2282,10 +2282,10 @@
       <c r="AH24" t="n">
         <v>0.05</v>
       </c>
-      <c r="AM24" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN24" t="b">
+      <c r="AM24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN24" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2313,10 +2313,10 @@
       <c r="AH25" t="n">
         <v>0.05</v>
       </c>
-      <c r="AM25" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN25" t="b">
+      <c r="AM25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN25" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2344,10 +2344,10 @@
       <c r="AH26" t="n">
         <v>0.05</v>
       </c>
-      <c r="AM26" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN26" t="b">
+      <c r="AM26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN26" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2375,10 +2375,10 @@
       <c r="AH27" t="n">
         <v>0.05</v>
       </c>
-      <c r="AM27" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN27" t="b">
+      <c r="AM27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN27" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2406,10 +2406,10 @@
       <c r="AH28" t="n">
         <v>0.05</v>
       </c>
-      <c r="AM28" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN28" t="b">
+      <c r="AM28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN28" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2437,10 +2437,10 @@
       <c r="AH29" t="n">
         <v>0.05</v>
       </c>
-      <c r="AM29" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN29" t="b">
+      <c r="AM29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN29" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2468,10 +2468,10 @@
       <c r="AH30" t="n">
         <v>0.05</v>
       </c>
-      <c r="AM30" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN30" t="b">
+      <c r="AM30" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN30" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2499,10 +2499,10 @@
       <c r="AH31" t="n">
         <v>0.05</v>
       </c>
-      <c r="AM31" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN31" t="b">
+      <c r="AM31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN31" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2530,10 +2530,10 @@
       <c r="AH32" t="n">
         <v>0.05</v>
       </c>
-      <c r="AM32" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN32" t="b">
+      <c r="AM32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN32" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2561,10 +2561,10 @@
       <c r="AH33" t="n">
         <v>0.05</v>
       </c>
-      <c r="AM33" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN33" t="b">
+      <c r="AM33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN33" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2592,10 +2592,10 @@
       <c r="AH34" t="n">
         <v>0.05</v>
       </c>
-      <c r="AM34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN34" t="b">
+      <c r="AM34" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN34" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2623,10 +2623,10 @@
       <c r="AH35" t="n">
         <v>0.05</v>
       </c>
-      <c r="AM35" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN35" t="b">
+      <c r="AM35" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN35" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2654,10 +2654,10 @@
       <c r="AH36" t="n">
         <v>0.05</v>
       </c>
-      <c r="AM36" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN36" t="b">
+      <c r="AM36" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN36" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2680,10 +2680,10 @@
       <c r="AH37" t="n">
         <v>0.0165</v>
       </c>
-      <c r="AM37" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN37" t="b">
+      <c r="AM37" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN37" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2706,10 +2706,10 @@
       <c r="AH38" t="n">
         <v>0.05</v>
       </c>
-      <c r="AM38" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN38" t="b">
+      <c r="AM38" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN38" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2732,10 +2732,10 @@
       <c r="AH39" t="n">
         <v>0.05</v>
       </c>
-      <c r="AM39" t="b">
+      <c r="AM39" t="n">
         <v>0</v>
       </c>
-      <c r="AN39" t="b">
+      <c r="AN39" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2763,10 +2763,10 @@
       <c r="AH40" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM40" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN40" t="b">
+      <c r="AM40" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN40" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2794,10 +2794,10 @@
       <c r="AH41" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM41" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN41" t="b">
+      <c r="AM41" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN41" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2825,10 +2825,10 @@
       <c r="AH42" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM42" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN42" t="b">
+      <c r="AM42" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN42" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2856,10 +2856,10 @@
       <c r="AH43" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM43" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN43" t="b">
+      <c r="AM43" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN43" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2887,10 +2887,10 @@
       <c r="AH44" t="n">
         <v>0.0979</v>
       </c>
-      <c r="AM44" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN44" t="b">
+      <c r="AM44" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN44" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2918,10 +2918,10 @@
       <c r="AH45" t="n">
         <v>0.0979</v>
       </c>
-      <c r="AM45" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN45" t="b">
+      <c r="AM45" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN45" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2944,12 +2944,6 @@
       <c r="AH46" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM46" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN46" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -2980,12 +2974,6 @@
       <c r="AH47" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM47" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN47" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -3016,12 +3004,6 @@
       <c r="AH48" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM48" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN48" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -3052,12 +3034,6 @@
       <c r="AH49" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM49" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN49" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -3088,12 +3064,6 @@
       <c r="AH50" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM50" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN50" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -3124,12 +3094,6 @@
       <c r="AH51" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM51" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN51" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -3160,12 +3124,6 @@
       <c r="AH52" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM52" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN52" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -3196,12 +3154,6 @@
       <c r="AH53" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM53" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN53" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -3232,12 +3184,6 @@
       <c r="AH54" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM54" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN54" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -3268,12 +3214,6 @@
       <c r="AH55" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM55" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN55" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -3304,12 +3244,6 @@
       <c r="AH56" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM56" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN56" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -3340,12 +3274,6 @@
       <c r="AH57" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM57" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN57" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -3376,12 +3304,6 @@
       <c r="AH58" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM58" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN58" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -3412,12 +3334,6 @@
       <c r="AH59" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM59" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN59" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -3448,12 +3364,6 @@
       <c r="AH60" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM60" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN60" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -3484,12 +3394,6 @@
       <c r="AH61" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM61" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN61" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -3520,12 +3424,6 @@
       <c r="AH62" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM62" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN62" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -3556,12 +3454,6 @@
       <c r="AH63" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM63" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN63" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -3592,12 +3484,6 @@
       <c r="AH64" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM64" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN64" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -3628,12 +3514,6 @@
       <c r="AH65" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM65" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN65" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -3664,12 +3544,6 @@
       <c r="AH66" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM66" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN66" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -3700,12 +3574,6 @@
       <c r="AH67" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM67" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN67" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -3736,12 +3604,6 @@
       <c r="AH68" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM68" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN68" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -3772,12 +3634,6 @@
       <c r="AH69" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM69" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN69" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -3808,12 +3664,6 @@
       <c r="AH70" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM70" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN70" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -3844,12 +3694,6 @@
       <c r="AH71" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM71" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN71" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -3880,12 +3724,6 @@
       <c r="AH72" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM72" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN72" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -3916,12 +3754,6 @@
       <c r="AH73" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM73" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN73" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -3952,12 +3784,6 @@
       <c r="AH74" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM74" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN74" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -3988,12 +3814,6 @@
       <c r="AH75" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM75" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN75" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -4024,12 +3844,6 @@
       <c r="AH76" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM76" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN76" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -4060,12 +3874,6 @@
       <c r="AH77" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM77" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN77" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -4096,12 +3904,6 @@
       <c r="AH78" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM78" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN78" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -4132,12 +3934,6 @@
       <c r="AH79" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM79" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN79" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -4168,12 +3964,6 @@
       <c r="AH80" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM80" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN80" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -4204,12 +3994,6 @@
       <c r="AH81" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM81" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN81" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -4240,12 +4024,6 @@
       <c r="AH82" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM82" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN82" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
@@ -4276,12 +4054,6 @@
       <c r="AH83" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM83" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN83" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -4312,12 +4084,6 @@
       <c r="AH84" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM84" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN84" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -4348,12 +4114,6 @@
       <c r="AH85" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM85" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN85" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -4384,12 +4144,6 @@
       <c r="AH86" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM86" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN86" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -4420,12 +4174,6 @@
       <c r="AH87" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM87" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN87" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -4451,12 +4199,6 @@
       <c r="AH88" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM88" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN88" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -4482,12 +4224,6 @@
       <c r="AH89" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM89" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN89" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -4513,12 +4249,6 @@
       <c r="AH90" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM90" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN90" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -4544,12 +4274,6 @@
       <c r="AH91" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM91" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN91" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -4575,12 +4299,6 @@
       <c r="AH92" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM92" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN92" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -4606,12 +4324,6 @@
       <c r="AH93" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM93" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN93" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -4637,12 +4349,6 @@
       <c r="AH94" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM94" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN94" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -4668,12 +4374,6 @@
       <c r="AH95" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM95" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN95" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -4699,12 +4399,6 @@
       <c r="AH96" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM96" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN96" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -4730,12 +4424,6 @@
       <c r="AH97" t="n">
         <v>0.1</v>
       </c>
-      <c r="AM97" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN97" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -4751,12 +4439,6 @@
         <v>0.3</v>
       </c>
       <c r="AH98" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM98" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN98" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>